<commit_message>
afwijking berekenen heeft een afwijking
de form opnieuw opbouwen voor hij in nieuw projekt wordt geplaatst
</commit_message>
<xml_diff>
--- a/source/file_in/202014342_proef.xlsx
+++ b/source/file_in/202014342_proef.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhr. Ten Hoonte\PycharmProjects\TC_mjth_2019\source\file_in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C47C484-A21D-4E91-AC8D-5C284938A5F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A8A6C78-65C7-455F-865A-5FE9D2E86F7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{4D8FFFBD-A8BD-6149-8204-48330D6B47B7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15375" windowHeight="20385" xr2:uid="{4D8FFFBD-A8BD-6149-8204-48330D6B47B7}"/>
   </bookViews>
   <sheets>
     <sheet name="202014342_proef" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="120">
   <si>
     <t>aantal</t>
   </si>
@@ -283,16 +283,130 @@
   </si>
   <si>
     <t>Colorcode</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>rolnum</t>
+  </si>
+  <si>
+    <t>Rol 1</t>
+  </si>
+  <si>
+    <t>Rol 7</t>
+  </si>
+  <si>
+    <t>Rol 8</t>
+  </si>
+  <si>
+    <t>Rol 2</t>
+  </si>
+  <si>
+    <t>Rol 3</t>
+  </si>
+  <si>
+    <t>Rol 4</t>
+  </si>
+  <si>
+    <t>Rol 5</t>
+  </si>
+  <si>
+    <t>Rol 6</t>
+  </si>
+  <si>
+    <t>Rol 9</t>
+  </si>
+  <si>
+    <t>Rol 10</t>
+  </si>
+  <si>
+    <t>Rol 11</t>
+  </si>
+  <si>
+    <t>Rol 12</t>
+  </si>
+  <si>
+    <t>Rol 13</t>
+  </si>
+  <si>
+    <t>Rol 14</t>
+  </si>
+  <si>
+    <t>Rol 15</t>
+  </si>
+  <si>
+    <t>Rol 16</t>
+  </si>
+  <si>
+    <t>Rol 17</t>
+  </si>
+  <si>
+    <t>Rol 18</t>
+  </si>
+  <si>
+    <t>Rol 19</t>
+  </si>
+  <si>
+    <t>Rol 20</t>
+  </si>
+  <si>
+    <t>Rol 21</t>
+  </si>
+  <si>
+    <t>Rol 22</t>
+  </si>
+  <si>
+    <t>Rol 23</t>
+  </si>
+  <si>
+    <t>Rol 24</t>
+  </si>
+  <si>
+    <t>Rol 25</t>
+  </si>
+  <si>
+    <t>Rol 26</t>
+  </si>
+  <si>
+    <t>Rol 27</t>
+  </si>
+  <si>
+    <t>Rol 28</t>
+  </si>
+  <si>
+    <t>Rol 29</t>
+  </si>
+  <si>
+    <t>Rol 30</t>
+  </si>
+  <si>
+    <t>Rol 31</t>
+  </si>
+  <si>
+    <t>Rol 32</t>
+  </si>
+  <si>
+    <t>Rol 33</t>
+  </si>
+  <si>
+    <t>Rol 34</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -634,10 +748,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{453506B7-7B18-4549-B992-CC4996C90829}">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J35"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -647,9 +761,10 @@
     <col min="5" max="5" width="17.25" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="34.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="43.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -678,10 +793,16 @@
         <v>48</v>
       </c>
       <c r="J1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>400</v>
       </c>
@@ -713,8 +834,15 @@
         <f>CONCATENATE(B2," | ",E2)</f>
         <v>White Out | LOT: 190114-1</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" t="str">
+        <f>CONCATENATE(L2," | ",J2)</f>
+        <v>Rol 1 | White Out | LOT: 190114-1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>200</v>
       </c>
@@ -746,8 +874,15 @@
         <f t="shared" ref="J3:J35" si="0">CONCATENATE(B3," | ",E3)</f>
         <v>Red Out | LOT: 190114-1</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K35" si="1">CONCATENATE(L3," | ",J3)</f>
+        <v>Rol 2 | Red Out | LOT: 190114-1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>200</v>
       </c>
@@ -779,8 +914,15 @@
         <f t="shared" si="0"/>
         <v>Contact lenses Out | LOT: 190114-1</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" t="str">
+        <f t="shared" si="1"/>
+        <v>Rol 3 | Contact lenses Out | LOT: 190114-1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>200</v>
       </c>
@@ -812,8 +954,15 @@
         <f t="shared" si="0"/>
         <v>Contact lenses Twilight  | LOT: 190114-1</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" t="str">
+        <f t="shared" si="1"/>
+        <v>Rol 4 | Contact lenses Twilight  | LOT: 190114-1</v>
+      </c>
+      <c r="L5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>200</v>
       </c>
@@ -845,8 +994,15 @@
         <f t="shared" si="0"/>
         <v>Magic Red | LOT: 190114-1</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" t="str">
+        <f t="shared" si="1"/>
+        <v>Rol 5 | Magic Red | LOT: 190114-1</v>
+      </c>
+      <c r="L6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>200</v>
       </c>
@@ -878,8 +1034,15 @@
         <f t="shared" si="0"/>
         <v>Magic Blue | LOT: 190114-1</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" t="str">
+        <f t="shared" si="1"/>
+        <v>Rol 6 | Magic Blue | LOT: 190114-1</v>
+      </c>
+      <c r="L7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>200</v>
       </c>
@@ -911,8 +1074,15 @@
         <f t="shared" si="0"/>
         <v>Magic Pink | LOT: 190114-1</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" t="str">
+        <f t="shared" si="1"/>
+        <v>Rol 7 | Magic Pink | LOT: 190114-1</v>
+      </c>
+      <c r="L8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>200</v>
       </c>
@@ -944,8 +1114,15 @@
         <f t="shared" si="0"/>
         <v>Contact lenses Magic | LOT: 190114-1</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" t="str">
+        <f t="shared" si="1"/>
+        <v>Rol 8 | Contact lenses Magic | LOT: 190114-1</v>
+      </c>
+      <c r="L9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>200</v>
       </c>
@@ -977,8 +1154,15 @@
         <f t="shared" si="0"/>
         <v>White Manson | LOT: 190114-1</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" t="str">
+        <f t="shared" si="1"/>
+        <v>Rol 9 | White Manson | LOT: 190114-1</v>
+      </c>
+      <c r="L10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>300</v>
       </c>
@@ -1010,8 +1194,15 @@
         <f t="shared" si="0"/>
         <v>Contact lenses Manson | LOT: 190114-1</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" t="str">
+        <f t="shared" si="1"/>
+        <v>Rol 10 | Contact lenses Manson | LOT: 190114-1</v>
+      </c>
+      <c r="L11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>200</v>
       </c>
@@ -1043,8 +1234,15 @@
         <f t="shared" si="0"/>
         <v>Red Manson | LOT: 190114-1</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" t="str">
+        <f t="shared" si="1"/>
+        <v>Rol 11 | Red Manson | LOT: 190114-1</v>
+      </c>
+      <c r="L12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>200</v>
       </c>
@@ -1076,8 +1274,15 @@
         <f t="shared" si="0"/>
         <v>Blood Drops | LOT: 190114-1</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" t="str">
+        <f t="shared" si="1"/>
+        <v>Rol 12 | Blood Drops | LOT: 190114-1</v>
+      </c>
+      <c r="L13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>200</v>
       </c>
@@ -1109,8 +1314,15 @@
         <f t="shared" si="0"/>
         <v>Contact lenses Wolf | LOT: 190114-1</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" t="str">
+        <f t="shared" si="1"/>
+        <v>Rol 13 | Contact lenses Wolf | LOT: 190114-1</v>
+      </c>
+      <c r="L14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>200</v>
       </c>
@@ -1142,8 +1354,15 @@
         <f t="shared" si="0"/>
         <v>Contact lenses Sharingan | LOT: 190114-1</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15" t="str">
+        <f t="shared" si="1"/>
+        <v>Rol 14 | Contact lenses Sharingan | LOT: 190114-1</v>
+      </c>
+      <c r="L15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>400</v>
       </c>
@@ -1175,8 +1394,15 @@
         <f t="shared" si="0"/>
         <v>Vampire red | LOT: 190114-1</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" t="str">
+        <f t="shared" si="1"/>
+        <v>Rol 15 | Vampire red | LOT: 190114-1</v>
+      </c>
+      <c r="L16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>200</v>
       </c>
@@ -1208,8 +1434,15 @@
         <f t="shared" si="0"/>
         <v>Vampire Green | LOT: 190114-1</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17" t="str">
+        <f t="shared" si="1"/>
+        <v>Rol 16 | Vampire Green | LOT: 190114-1</v>
+      </c>
+      <c r="L17" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>200</v>
       </c>
@@ -1241,8 +1474,15 @@
         <f t="shared" si="0"/>
         <v>Contact lenses Vampire | LOT: 190114-1</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" t="str">
+        <f t="shared" si="1"/>
+        <v>Rol 17 | Contact lenses Vampire | LOT: 190114-1</v>
+      </c>
+      <c r="L18" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>200</v>
       </c>
@@ -1274,8 +1514,15 @@
         <f t="shared" si="0"/>
         <v>Shiny Blue | LOT: 190114-1</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" t="str">
+        <f t="shared" si="1"/>
+        <v>Rol 18 | Shiny Blue | LOT: 190114-1</v>
+      </c>
+      <c r="L19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>200</v>
       </c>
@@ -1307,8 +1554,15 @@
         <f t="shared" si="0"/>
         <v>Contact lenses Shiny | LOT: 190114-1</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20" t="str">
+        <f t="shared" si="1"/>
+        <v>Rol 19 | Contact lenses Shiny | LOT: 190114-1</v>
+      </c>
+      <c r="L20" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1500</v>
       </c>
@@ -1337,8 +1591,15 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> | LOT: 190114-1</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" t="str">
+        <f t="shared" si="1"/>
+        <v>Rol 20 |  | LOT: 190114-1</v>
+      </c>
+      <c r="L21" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>200</v>
       </c>
@@ -1370,8 +1631,15 @@
         <f t="shared" si="0"/>
         <v>Contact lenses Aqua | LOT: 190724-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22" t="str">
+        <f t="shared" si="1"/>
+        <v>Rol 21 | Contact lenses Aqua | LOT: 190724-2</v>
+      </c>
+      <c r="L22" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>200</v>
       </c>
@@ -1403,8 +1671,15 @@
         <f t="shared" si="0"/>
         <v>Contact lenses Twist  | LOT: 190724-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" t="str">
+        <f t="shared" si="1"/>
+        <v>Rol 22 | Contact lenses Twist  | LOT: 190724-2</v>
+      </c>
+      <c r="L23" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>200</v>
       </c>
@@ -1436,8 +1711,15 @@
         <f t="shared" si="0"/>
         <v>Contact lenses Clear | LOT: 190724-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24" t="str">
+        <f t="shared" si="1"/>
+        <v>Rol 23 | Contact lenses Clear | LOT: 190724-2</v>
+      </c>
+      <c r="L24" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>200</v>
       </c>
@@ -1469,8 +1751,15 @@
         <f t="shared" si="0"/>
         <v>Clear Green | LOT: 190724-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" t="str">
+        <f t="shared" si="1"/>
+        <v>Rol 24 | Clear Green | LOT: 190724-2</v>
+      </c>
+      <c r="L25" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>200</v>
       </c>
@@ -1502,8 +1791,15 @@
         <f t="shared" si="0"/>
         <v>Contact lenses Glamour | LOT: 190724-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26" t="str">
+        <f t="shared" si="1"/>
+        <v>Rol 25 | Contact lenses Glamour | LOT: 190724-2</v>
+      </c>
+      <c r="L26" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>200</v>
       </c>
@@ -1535,8 +1831,15 @@
         <f t="shared" si="0"/>
         <v>Contact lenses Dots   | LOT: 190724-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K27" t="str">
+        <f t="shared" si="1"/>
+        <v>Rol 26 | Contact lenses Dots   | LOT: 190724-2</v>
+      </c>
+      <c r="L27" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>200</v>
       </c>
@@ -1568,8 +1871,15 @@
         <f t="shared" si="0"/>
         <v>Contact lenses Glossy  | LOT: 190724-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K28" t="str">
+        <f t="shared" si="1"/>
+        <v>Rol 27 | Contact lenses Glossy  | LOT: 190724-2</v>
+      </c>
+      <c r="L28" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>200</v>
       </c>
@@ -1601,8 +1911,15 @@
         <f t="shared" si="0"/>
         <v>Green Passion | LOT: 190724-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K29" t="str">
+        <f t="shared" si="1"/>
+        <v>Rol 28 | Green Passion | LOT: 190724-2</v>
+      </c>
+      <c r="L29" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>200</v>
       </c>
@@ -1634,8 +1951,15 @@
         <f t="shared" si="0"/>
         <v>Contact lenses Passion | LOT: 190724-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K30" t="str">
+        <f t="shared" si="1"/>
+        <v>Rol 29 | Contact lenses Passion | LOT: 190724-2</v>
+      </c>
+      <c r="L30" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>200</v>
       </c>
@@ -1667,8 +1991,15 @@
         <f t="shared" si="0"/>
         <v>Contact lenses Waves | LOT: 190724-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K31" t="str">
+        <f t="shared" si="1"/>
+        <v>Rol 30 | Contact lenses Waves | LOT: 190724-2</v>
+      </c>
+      <c r="L31" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>100</v>
       </c>
@@ -1700,8 +2031,15 @@
         <f t="shared" si="0"/>
         <v>Brown Waves | LOT: 190724-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K32" t="str">
+        <f t="shared" si="1"/>
+        <v>Rol 31 | Brown Waves | LOT: 190724-2</v>
+      </c>
+      <c r="L32" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1500</v>
       </c>
@@ -1730,8 +2068,15 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> | LOT: 190724-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K33" t="str">
+        <f t="shared" si="1"/>
+        <v>Rol 32 |  | LOT: 190724-2</v>
+      </c>
+      <c r="L33" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2600</v>
       </c>
@@ -1760,8 +2105,15 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> | LOT: 200826-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K34" t="str">
+        <f t="shared" si="1"/>
+        <v>Rol 33 |  | LOT: 200826-2</v>
+      </c>
+      <c r="L34" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>500</v>
       </c>
@@ -1784,8 +2136,16 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve"> | Yearly Replacement</v>
       </c>
+      <c r="K35" t="str">
+        <f t="shared" si="1"/>
+        <v>Rol 34 |  | Yearly Replacement</v>
+      </c>
+      <c r="L35" t="s">
+        <v>119</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>